<commit_message>
Add tests for auth form
</commit_message>
<xml_diff>
--- a/chek-list.xlsx
+++ b/chek-list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Чек-лист</t>
   </si>
@@ -69,16 +69,6 @@
     <t>С валидными данными пользователя для авторизации:  testcaseqa5@gmail.com | 123456</t>
   </si>
   <si>
-    <t>С не валидными паролем пользователя для авторизации:  testcaseqa5@gmail.com | 4321</t>
-  </si>
-  <si>
-    <t>С не валидными логином пользователя:  testcaseqa5@gmail.com | 4321</t>
-  </si>
-  <si>
-    <t>С не валидными логином пользователя и не валидным паролем: 
- testcaseqa5@gmail.com | 4321</t>
-  </si>
-  <si>
     <t>Обновление личной информации пользователя</t>
   </si>
   <si>
@@ -95,6 +85,19 @@
   </si>
   <si>
     <t>Именить Business segment; Phone number : +7 4954434343</t>
+  </si>
+  <si>
+    <t>С ошибочным паролем пользователя для авторизации:  testcaseqa5@gmail.com | 4321</t>
+  </si>
+  <si>
+    <t>С ошибочным логином пользователя:  testcaseqa5@ | 123456</t>
+  </si>
+  <si>
+    <t>С ошибочным логином пользователя:  testcaseqa4@gmail.com | 123456</t>
+  </si>
+  <si>
+    <t>С ошибочным логином и паролем пользователя: 
+ testcaseqa3@gmail.com | 4321</t>
   </si>
 </sst>
 </file>
@@ -282,27 +285,6 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -318,21 +300,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -615,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:D24"/>
+  <dimension ref="B4:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,166 +633,173 @@
   <sheetData>
     <row r="4" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="2:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="B7" s="7"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="19" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="20" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-    </row>
-    <row r="14" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-    </row>
-    <row r="15" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="12" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-    </row>
-    <row r="16" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="12" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-    </row>
-    <row r="17" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-    </row>
-    <row r="19" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="12" t="s">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-    </row>
-    <row r="20" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-    </row>
-    <row r="21" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="12" t="s">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="12" t="s">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C23" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D23" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="15" t="s">
+    <row r="24" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C24" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D24" s="19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+    <row r="25" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="18"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B23:B24" r:id="rId1" display="https://www.flickr.com/photos/132666002@N02/19114395498"/>
+    <hyperlink ref="B24:B25" r:id="rId1" display="https://www.flickr.com/photos/132666002@N02/19114395498"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Added tests for change profile.Created bug_reports.
</commit_message>
<xml_diff>
--- a/chek-list.xlsx
+++ b/chek-list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
   <si>
     <t>Чек-лист</t>
   </si>
@@ -44,25 +44,6 @@
     <t>pass</t>
   </si>
   <si>
-    <t>Задача не выполнена</t>
-  </si>
-  <si>
-    <t>Графический интерфей</t>
-  </si>
-  <si>
-    <t>Отображаются все задачи, которые создали.</t>
-  </si>
-  <si>
-    <t>Все задачи разбиты на категории</t>
-  </si>
-  <si>
-    <t>Верстка соответствует эскизам
-(https://www.flickr.com/photos/132666002@N02/19114395498)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fail bug#7, bug#8 </t>
-  </si>
-  <si>
     <t>Авторизация пользователя</t>
   </si>
   <si>
@@ -76,9 +57,6 @@
   </si>
   <si>
     <t>Именить Country: Russia; Phone number : +7 4954434343</t>
-  </si>
-  <si>
-    <t>Именить User name; Phone number : +7 4954434343</t>
   </si>
   <si>
     <t>Именить email address: testcaseqa@gmail.com; Phone number : +7 4954434343</t>
@@ -98,13 +76,25 @@
   <si>
     <t>С ошибочным логином и паролем пользователя: 
  testcaseqa3@gmail.com | 4321</t>
+  </si>
+  <si>
+    <t>Именить User name : Alex_323 ; Phone number : +7 4954434343</t>
+  </si>
+  <si>
+    <t>Именить email address: testcaseqa.com; Phone number : +7 4954434343</t>
+  </si>
+  <si>
+    <t>Именить Phone number на не валидный: +7 3343524334332</t>
+  </si>
+  <si>
+    <t>fail bug#1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,15 +128,6 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -168,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -265,25 +246,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,14 +259,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -325,21 +288,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -618,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:D25"/>
+  <dimension ref="B4:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -633,23 +583,23 @@
   <sheetData>
     <row r="4" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="2:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
@@ -659,149 +609,162 @@
     </row>
     <row r="8" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="D10" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="B13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="B16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="C18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="18"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-    </row>
+      <c r="C21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="3">
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B24:B25" r:id="rId1" display="https://www.flickr.com/photos/132666002@N02/19114395498"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>